<commit_message>
Updated the excel document
</commit_message>
<xml_diff>
--- a/Move mid-terms and project #1 dates.xlsx
+++ b/Move mid-terms and project #1 dates.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A7804-C510-49B0-974D-DC6D482B973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5125C99B-F9B5-4A3D-96E4-C138FA6EA3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>1194316</t>
   </si>
@@ -56,9 +59,6 @@
   </si>
   <si>
     <t>1266871</t>
-  </si>
-  <si>
-    <t>1252675</t>
   </si>
   <si>
     <t>1278993</t>
@@ -225,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +403,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -581,7 +587,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,14 +598,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -648,6 +657,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF66"/>
+      <color rgb="FF99FFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -976,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77382190-FC37-4831-B9FD-F32C05751A68}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A20" sqref="A20:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,24 +1004,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="6"/>
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1014,15 +1029,15 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1030,7 +1045,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1039,7 +1054,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,97 +1062,86 @@
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5"/>
+      <c r="B19" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B17">
-    <sortCondition ref="A4:A17"/>
-  </sortState>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A4:A17" numberStoredAsText="1"/>
+    <ignoredError sqref="A4:A9 A10:A16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>